<commit_message>
Forgot to add excel file modifications
</commit_message>
<xml_diff>
--- a/Scripts/benchmark_template.xlsx
+++ b/Scripts/benchmark_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quinc\Documents\UF\UF_FALL_2024\Computer Engineering Design 1\AI-Edge-Benchmarking\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3305A714-3A1B-4D68-98D1-31F95E712D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A792E4CE-36F8-40C0-BE28-6E26FC5DF466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0DDF3B5D-B2B5-49C0-93F1-AEDB294FEFA2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Name of current trial for the board</t>
+  </si>
+  <si>
+    <t>Number of measurements for taking idle current</t>
+  </si>
+  <si>
+    <t>idle_iterations</t>
   </si>
 </sst>
 </file>
@@ -366,6 +372,9 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -379,9 +388,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -443,8 +449,8 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9A256627-9EDB-4CF1-B3AA-2EF08CC035C8}" name="Description" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{15B6806D-36A6-4040-BDFB-83EF9129A011}" name="Name" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{A5728122-5DA9-4717-A0CF-BCB39D255380}" name="Value" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{8B2A0ED2-0E33-4DA0-A34B-DE44E4093DE3}" name="Flag" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{A5728122-5DA9-4717-A0CF-BCB39D255380}" name="Value" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{8B2A0ED2-0E33-4DA0-A34B-DE44E4093DE3}" name="Flag" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -767,11 +773,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AB1A43-3FAF-434F-B16F-E752B5AD3176}">
-  <dimension ref="A1:HR12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -947,6 +953,18 @@
       </c>
       <c r="D12" s="11"/>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="14">
+        <v>20</v>
+      </c>
+      <c r="D13" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>